<commit_message>
feature: credential changed to dev account
</commit_message>
<xml_diff>
--- a/xlsx/2023/2/2023-02-20~2023-02-26.xlsx
+++ b/xlsx/2023/2/2023-02-20~2023-02-26.xlsx
@@ -523,11 +523,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="576737516"/>
-        <c:axId val="1829104869"/>
+        <c:axId val="539783490"/>
+        <c:axId val="1982131615"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="576737516"/>
+        <c:axId val="539783490"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,10 +579,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1829104869"/>
+        <c:crossAx val="1982131615"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1829104869"/>
+        <c:axId val="1982131615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576737516"/>
+        <c:crossAx val="539783490"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -787,11 +787,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1224121738"/>
-        <c:axId val="89130604"/>
+        <c:axId val="1134929994"/>
+        <c:axId val="975888320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1224121738"/>
+        <c:axId val="1134929994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,10 +843,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89130604"/>
+        <c:crossAx val="975888320"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89130604"/>
+        <c:axId val="975888320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +921,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1224121738"/>
+        <c:crossAx val="1134929994"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1051,11 +1051,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1325477642"/>
-        <c:axId val="1565645110"/>
+        <c:axId val="460627329"/>
+        <c:axId val="81058303"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1325477642"/>
+        <c:axId val="460627329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,10 +1107,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1565645110"/>
+        <c:crossAx val="81058303"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1565645110"/>
+        <c:axId val="81058303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +1185,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1325477642"/>
+        <c:crossAx val="460627329"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1315,11 +1315,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1138884671"/>
-        <c:axId val="181617024"/>
+        <c:axId val="780514031"/>
+        <c:axId val="1542153829"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1138884671"/>
+        <c:axId val="780514031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,10 +1371,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181617024"/>
+        <c:crossAx val="1542153829"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181617024"/>
+        <c:axId val="1542153829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1449,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1138884671"/>
+        <c:crossAx val="780514031"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1579,11 +1579,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1105385003"/>
-        <c:axId val="481118981"/>
+        <c:axId val="1892093731"/>
+        <c:axId val="702926272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1105385003"/>
+        <c:axId val="1892093731"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,10 +1635,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="481118981"/>
+        <c:crossAx val="702926272"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="481118981"/>
+        <c:axId val="702926272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1713,7 +1713,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1105385003"/>
+        <c:crossAx val="1892093731"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1843,11 +1843,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="301230319"/>
-        <c:axId val="1092163978"/>
+        <c:axId val="441238452"/>
+        <c:axId val="1535992506"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="301230319"/>
+        <c:axId val="441238452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,10 +1899,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1092163978"/>
+        <c:crossAx val="1535992506"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1092163978"/>
+        <c:axId val="1535992506"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1977,7 +1977,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301230319"/>
+        <c:crossAx val="441238452"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2107,11 +2107,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1741499"/>
-        <c:axId val="1907023461"/>
+        <c:axId val="1527333655"/>
+        <c:axId val="1492081144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1741499"/>
+        <c:axId val="1527333655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,10 +2163,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1907023461"/>
+        <c:crossAx val="1492081144"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1907023461"/>
+        <c:axId val="1492081144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,7 +2241,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1741499"/>
+        <c:crossAx val="1527333655"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2371,11 +2371,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="638602737"/>
-        <c:axId val="185826599"/>
+        <c:axId val="1253280304"/>
+        <c:axId val="1079169499"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="638602737"/>
+        <c:axId val="1253280304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,10 +2427,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185826599"/>
+        <c:crossAx val="1079169499"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185826599"/>
+        <c:axId val="1079169499"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2505,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="638602737"/>
+        <c:crossAx val="1253280304"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2684,11 +2684,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1111320520"/>
-        <c:axId val="28198527"/>
+        <c:axId val="322587847"/>
+        <c:axId val="1199843090"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1111320520"/>
+        <c:axId val="322587847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,10 +2740,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28198527"/>
+        <c:crossAx val="1199843090"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28198527"/>
+        <c:axId val="1199843090"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2818,7 +2818,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1111320520"/>
+        <c:crossAx val="322587847"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2997,11 +2997,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1913605592"/>
-        <c:axId val="1342485709"/>
+        <c:axId val="616692321"/>
+        <c:axId val="338357394"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1913605592"/>
+        <c:axId val="616692321"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3053,10 +3053,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1342485709"/>
+        <c:crossAx val="338357394"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1342485709"/>
+        <c:axId val="338357394"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3131,7 +3131,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913605592"/>
+        <c:crossAx val="616692321"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3261,11 +3261,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="548679779"/>
-        <c:axId val="10108986"/>
+        <c:axId val="1200154899"/>
+        <c:axId val="465174932"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="548679779"/>
+        <c:axId val="1200154899"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3317,10 +3317,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10108986"/>
+        <c:crossAx val="465174932"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10108986"/>
+        <c:axId val="465174932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3395,7 +3395,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="548679779"/>
+        <c:crossAx val="1200154899"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3525,11 +3525,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1556729590"/>
-        <c:axId val="771289099"/>
+        <c:axId val="1777405083"/>
+        <c:axId val="1302099672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1556729590"/>
+        <c:axId val="1777405083"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,10 +3581,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="771289099"/>
+        <c:crossAx val="1302099672"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="771289099"/>
+        <c:axId val="1302099672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3659,7 +3659,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1556729590"/>
+        <c:crossAx val="1777405083"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3789,11 +3789,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1912584609"/>
-        <c:axId val="1770148620"/>
+        <c:axId val="79925088"/>
+        <c:axId val="1218619234"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1912584609"/>
+        <c:axId val="79925088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3845,10 +3845,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1770148620"/>
+        <c:crossAx val="1218619234"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1770148620"/>
+        <c:axId val="1218619234"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3923,7 +3923,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1912584609"/>
+        <c:crossAx val="79925088"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>